<commit_message>
estrutura de pastas script json
</commit_message>
<xml_diff>
--- a/scripts/Monitoramento/inputs/0 - Belém/0 - Monitoramento Form 1, 2 e 3.xlsx
+++ b/scripts/Monitoramento/inputs/0 - Belém/0 - Monitoramento Form 1, 2 e 3.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29602"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_B2111171719633AE9B1A26FD83EA69EFE7605594" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_8E812C7661EE4425CA297AF95453F10A4ACC2D56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -206,14 +206,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF006400"/>
-        <bgColor rgb="FF006400"/>
+        <fgColor rgb="FF66FF66"/>
+        <bgColor rgb="FF66FF66"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF66FF66"/>
-        <bgColor rgb="FF66FF66"/>
+        <fgColor rgb="FF006400"/>
+        <bgColor rgb="FF006400"/>
       </patternFill>
     </fill>
   </fills>
@@ -265,16 +265,13 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -284,6 +281,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -947,133 +947,133 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7" t="str">
+      <c r="B2" s="6" t="str">
         <f>COUNTIF(INDIRECT("'Form 1 - Município'!E2:E100"),"Enviado")</f>
         <v/>
       </c>
-      <c r="C2" s="8" t="str">
+      <c r="C2" s="7" t="str">
         <f>B2/SUM($B2,$D2,$F2)</f>
         <v/>
       </c>
-      <c r="D2" s="7" t="str">
+      <c r="D2" s="6" t="str">
         <f>COUNTIF(INDIRECT("'Form 1 - Município'!E2:E100"),"Atrasado")</f>
         <v/>
       </c>
-      <c r="E2" s="8" t="str">
+      <c r="E2" s="7" t="str">
         <f>D2/SUM($B2,$D2,$F2)</f>
         <v/>
       </c>
-      <c r="F2" s="7" t="str">
+      <c r="F2" s="6" t="str">
         <f>COUNTIF(INDIRECT("'Form 1 - Município'!E2:E100"),"Sem Técnico")</f>
         <v/>
       </c>
-      <c r="G2" s="8" t="str">
+      <c r="G2" s="7" t="str">
         <f>F2/SUM($B2,$D2,$F2)</f>
         <v/>
       </c>
-      <c r="H2" s="9" t="str">
+      <c r="H2" s="8" t="str">
         <f>SUM(B2,D2,F2)</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="str">
+      <c r="B3" s="6" t="str">
         <f>COUNTIF(INDIRECT("'Form 2 - UVR'!E2:E100"),"Enviado")</f>
         <v/>
       </c>
-      <c r="C3" s="8" t="str">
+      <c r="C3" s="7" t="str">
         <f>B3/SUM($B3,$D3,$F3)</f>
         <v/>
       </c>
-      <c r="D3" s="7" t="str">
+      <c r="D3" s="6" t="str">
         <f>COUNTIF(INDIRECT("'Form 2 - UVR'!E2:E100"),"Atrasado")</f>
         <v/>
       </c>
-      <c r="E3" s="8" t="str">
+      <c r="E3" s="7" t="str">
         <f>D3/SUM($B3,$D3,$F3)</f>
         <v/>
       </c>
-      <c r="F3" s="7" t="str">
+      <c r="F3" s="6" t="str">
         <f>COUNTIF(INDIRECT("'Form 2 - UVR'!E2:E100"),"Sem Técnico")</f>
         <v/>
       </c>
-      <c r="G3" s="8" t="str">
+      <c r="G3" s="7" t="str">
         <f>F3/SUM($B3,$D3,$F3)</f>
         <v/>
       </c>
-      <c r="H3" s="9" t="str">
+      <c r="H3" s="8" t="str">
         <f>SUM(B3,D3,F3)</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="7" t="str">
+      <c r="B4" s="6" t="str">
         <f>COUNTIF(INDIRECT("'Form 3 - Empreendimento'!E2:E100"),"Enviado")</f>
         <v/>
       </c>
-      <c r="C4" s="8" t="str">
+      <c r="C4" s="7" t="str">
         <f>B4/SUM($B4,$D4,$F4)</f>
         <v/>
       </c>
-      <c r="D4" s="7" t="str">
+      <c r="D4" s="6" t="str">
         <f>COUNTIF(INDIRECT("'Form 3 - Empreendimento'!E2:E100"),"Atrasado")</f>
         <v/>
       </c>
-      <c r="E4" s="8" t="str">
+      <c r="E4" s="7" t="str">
         <f>D4/SUM($B4,$D4,$F4)</f>
         <v/>
       </c>
-      <c r="F4" s="7" t="str">
+      <c r="F4" s="6" t="str">
         <f>COUNTIF(INDIRECT("'Form 3 - Empreendimento'!E2:E100"),"Sem Técnico")</f>
         <v/>
       </c>
-      <c r="G4" s="8" t="str">
+      <c r="G4" s="7" t="str">
         <f>F4/SUM($B4,$D4,$F4)</f>
         <v/>
       </c>
-      <c r="H4" s="9" t="str">
+      <c r="H4" s="8" t="str">
         <f>SUM(B4,D4,F4)</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="str">
+      <c r="B5" s="8" t="str">
         <f>SUM(B2:B4)</f>
         <v/>
       </c>
-      <c r="C5" s="8" t="str">
+      <c r="C5" s="7" t="str">
         <f>B5/SUM($B5,$D5,$F5)</f>
         <v/>
       </c>
-      <c r="D5" s="9" t="str">
+      <c r="D5" s="8" t="str">
         <f>SUM(D2:D4)</f>
         <v/>
       </c>
-      <c r="E5" s="8" t="str">
+      <c r="E5" s="7" t="str">
         <f>D5/SUM($B5,$D5,$F5)</f>
         <v/>
       </c>
-      <c r="F5" s="9" t="str">
+      <c r="F5" s="8" t="str">
         <f>SUM(F2:F4)</f>
         <v/>
       </c>
-      <c r="G5" s="8" t="str">
+      <c r="G5" s="7" t="str">
         <f>F5/SUM($B5,$D5,$F5)</f>
         <v/>
       </c>
-      <c r="H5" s="9" t="str">
+      <c r="H5" s="8" t="str">
         <f>SUM(B5,D5,F5)</f>
         <v/>
       </c>
@@ -1142,120 +1142,120 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="4"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="4"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
@@ -1369,124 +1369,124 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="str">
+      <c r="D2" s="3" t="str">
         <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B2&amp;C2, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B2&amp;C2, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
         <v/>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="4"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="str">
+      <c r="D3" s="3" t="str">
         <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B3&amp;C3, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B3&amp;C3, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
         <v/>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="str">
+      <c r="D4" s="3" t="str">
         <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B4&amp;C4, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B4&amp;C4, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
         <v/>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="4"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="str">
+      <c r="D5" s="3" t="str">
         <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B5&amp;C5, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B5&amp;C5, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
         <v/>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -1600,124 +1600,124 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="str">
+      <c r="D2" s="3" t="str">
         <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B2&amp;C2, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B2&amp;C2, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
         <v/>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="4"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="str">
+      <c r="D3" s="3" t="str">
         <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B3&amp;C3, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B3&amp;C3, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
         <v/>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="str">
+      <c r="D4" s="3" t="str">
         <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B4&amp;C4, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B4&amp;C4, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
         <v/>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="4"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="str">
+      <c r="D5" s="3" t="str">
         <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B5&amp;C5, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B5&amp;C5, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
         <v/>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>

</xml_diff>